<commit_message>
Updated function names and data documentation
</commit_message>
<xml_diff>
--- a/_health/fivestate/R/Params_US_5_state.xlsx
+++ b/_health/fivestate/R/Params_US_5_state.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxin/Dropbox/Year7/RA_Health_State/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxin/Documents/GitHub/retirement-toolkit/_health/fivestate/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A435AB-D0C2-3F4B-98A7-CDF8E607BBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4528ADD6-16D6-DC48-B418-4C4427E2B981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="1260" windowWidth="28040" windowHeight="17440" xr2:uid="{791C2F50-38CB-3540-B68D-030DFFC98AD7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>beta</t>
   </si>
@@ -51,16 +51,55 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>No frailty</t>
-  </si>
-  <si>
-    <t>No frailty with trend</t>
-  </si>
-  <si>
     <t>Frailty</t>
   </si>
   <si>
-    <t>transition type s</t>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Coef</t>
+  </si>
+  <si>
+    <t>trans1</t>
+  </si>
+  <si>
+    <t>trans2</t>
+  </si>
+  <si>
+    <t>trans3</t>
+  </si>
+  <si>
+    <t>trans4</t>
+  </si>
+  <si>
+    <t>trans5</t>
+  </si>
+  <si>
+    <t>trans6</t>
+  </si>
+  <si>
+    <t>trans7</t>
+  </si>
+  <si>
+    <t>trans8</t>
+  </si>
+  <si>
+    <t>trans9</t>
+  </si>
+  <si>
+    <t>trans10</t>
+  </si>
+  <si>
+    <t>trans11</t>
+  </si>
+  <si>
+    <t>trans12</t>
+  </si>
+  <si>
+    <t>Trend</t>
   </si>
 </sst>
 </file>
@@ -68,12 +107,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,9 +464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CA97C1-5146-364A-9822-6336C7ED3F90}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -430,49 +477,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
+      <c r="F1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -515,6 +565,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -556,6 +609,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -597,409 +653,403 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-4.8564999999999996</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-9.8825000000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-12.2934</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-11.1325</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-7.2309000000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-9.2922999999999991</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.4042</v>
+      </c>
+      <c r="J5" s="2">
+        <v>-1.9753000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-4.3003</v>
+      </c>
+      <c r="L5" s="2">
+        <v>-7.9431000000000003</v>
+      </c>
+      <c r="M5" s="2">
+        <v>-1.55E-2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>-6.2411000000000003</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.1042</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-3.1699999999999999E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-2.18E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>-3.0700000000000002E-2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5.8799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.3201</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.26829999999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-0.55100000000000005</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.38369999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-0.2702</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>-0.16880000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="L7" s="2">
+        <v>-0.46500000000000002</v>
+      </c>
+      <c r="M7" s="2">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>-0.31390000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-4.7500000000000001E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-5.5800000000000002E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-7.2099999999999997E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-2.8199999999999999E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-7.1900000000000006E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>-1.2800000000000001E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L8" s="2">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1.01E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>-1.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
-        <v>-4.8564999999999996</v>
-      </c>
-      <c r="D6" s="2">
-        <v>-9.8825000000000003</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-12.2934</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-11.1325</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-7.2309000000000001</v>
-      </c>
-      <c r="H6" s="2">
-        <v>-9.2922999999999991</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.4042</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-1.9753000000000001</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-4.3003</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-7.9431000000000003</v>
-      </c>
-      <c r="M6" s="2">
-        <v>-1.55E-2</v>
-      </c>
-      <c r="N6" s="2">
-        <v>-6.2411000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="C9" s="2">
+        <v>-4.8818999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-9.8857999999999997</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-12.2858</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-11.1111</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-7.2375999999999996</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-9.2752999999999997</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.4088</v>
+      </c>
+      <c r="J9" s="2">
+        <v>-1.9761</v>
+      </c>
+      <c r="K9" s="2">
+        <v>-4.3011999999999997</v>
+      </c>
+      <c r="L9" s="2">
+        <v>-7.9530000000000003</v>
+      </c>
+      <c r="M9" s="2">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>-6.2489999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2">
-        <v>2.5100000000000001E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7.9299999999999995E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>9.6500000000000002E-2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.1042</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="C10" s="2">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9.7900000000000001E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.10390000000000001</v>
+      </c>
+      <c r="G10" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H7" s="2">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>-3.1699999999999999E-2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>-2.18E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="H10" s="2">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-3.1199999999999999E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>-1.95E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.47E-2</v>
+      </c>
+      <c r="L10" s="2">
         <v>7.4099999999999999E-2</v>
       </c>
-      <c r="M7" s="2">
-        <v>-3.0700000000000002E-2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>5.8799999999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-0.3201</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.26829999999999998</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.14030000000000001</v>
-      </c>
-      <c r="F8" s="2">
-        <v>-0.55100000000000005</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.38369999999999999</v>
-      </c>
-      <c r="H8" s="2">
-        <v>-0.2702</v>
-      </c>
-      <c r="I8" s="2">
-        <v>-3.2000000000000001E-2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>-0.16880000000000001</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.14580000000000001</v>
-      </c>
-      <c r="L8" s="2">
-        <v>-0.46500000000000002</v>
-      </c>
-      <c r="M8" s="2">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="N8" s="2">
-        <v>-0.31390000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-4.7500000000000001E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-5.5800000000000002E-2</v>
-      </c>
-      <c r="F9" s="2">
-        <v>-7.2099999999999997E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <v>-2.8199999999999999E-2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>-7.1900000000000006E-2</v>
-      </c>
-      <c r="I9" s="2">
-        <v>-1.2800000000000001E-2</v>
-      </c>
-      <c r="J9" s="2">
-        <v>-2.1999999999999999E-2</v>
-      </c>
-      <c r="K9" s="2">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="L9" s="2">
-        <v>-9.1999999999999998E-3</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1.01E-2</v>
-      </c>
-      <c r="N9" s="2">
-        <v>-1.8200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="M10" s="2">
+        <v>-0.03</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5.91E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>-4.8818999999999999</v>
+        <v>-0.32340000000000002</v>
       </c>
       <c r="D11" s="2">
-        <v>-9.8857999999999997</v>
+        <v>0.2712</v>
       </c>
       <c r="E11" s="2">
-        <v>-12.2858</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="F11" s="2">
-        <v>-11.1111</v>
+        <v>-0.54620000000000002</v>
       </c>
       <c r="G11" s="2">
-        <v>-7.2375999999999996</v>
+        <v>0.38519999999999999</v>
       </c>
       <c r="H11" s="2">
-        <v>-9.2752999999999997</v>
+        <v>-0.2676</v>
       </c>
       <c r="I11" s="2">
-        <v>0.4088</v>
+        <v>-0.03</v>
       </c>
       <c r="J11" s="2">
-        <v>-1.9761</v>
+        <v>-0.16950000000000001</v>
       </c>
       <c r="K11" s="2">
-        <v>-4.3011999999999997</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="L11" s="2">
-        <v>-7.9530000000000003</v>
+        <v>-0.4672</v>
       </c>
       <c r="M11" s="2">
-        <v>-1.4999999999999999E-2</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="N11" s="2">
-        <v>-6.2489999999999997</v>
+        <v>-0.31609999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>2.5399999999999999E-2</v>
+        <v>3.2800000000000003E-2</v>
       </c>
       <c r="D12" s="2">
-        <v>7.9200000000000007E-2</v>
+        <v>-4.2700000000000002E-2</v>
       </c>
       <c r="E12" s="2">
-        <v>9.7900000000000001E-2</v>
+        <v>-9.0800000000000006E-2</v>
       </c>
       <c r="F12" s="2">
-        <v>0.10390000000000001</v>
+        <v>-7.1499999999999994E-2</v>
       </c>
       <c r="G12" s="2">
-        <v>5.3999999999999999E-2</v>
+        <v>-2.69E-2</v>
       </c>
       <c r="H12" s="2">
-        <v>8.7499999999999994E-2</v>
+        <v>-6.4299999999999996E-2</v>
       </c>
       <c r="I12" s="2">
-        <v>-3.1199999999999999E-2</v>
+        <v>-2.9600000000000001E-2</v>
       </c>
       <c r="J12" s="2">
-        <v>-1.95E-2</v>
+        <v>-6.9099999999999995E-2</v>
       </c>
       <c r="K12" s="2">
-        <v>1.47E-2</v>
+        <v>-1.35E-2</v>
       </c>
       <c r="L12" s="2">
-        <v>7.4099999999999999E-2</v>
+        <v>-4.1000000000000003E-3</v>
       </c>
       <c r="M12" s="2">
-        <v>-0.03</v>
+        <v>-1.15E-2</v>
       </c>
       <c r="N12" s="2">
-        <v>5.91E-2</v>
+        <v>-2.3800000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>-0.32340000000000002</v>
+        <v>-1.0800000000000001E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.2712</v>
+        <v>-2.35E-2</v>
       </c>
       <c r="E13" s="2">
-        <v>0.14580000000000001</v>
+        <v>4.5400000000000003E-2</v>
       </c>
       <c r="F13" s="2">
-        <v>-0.54620000000000002</v>
+        <v>-1.4E-3</v>
       </c>
       <c r="G13" s="2">
-        <v>0.38519999999999999</v>
+        <v>-5.7999999999999996E-3</v>
       </c>
       <c r="H13" s="2">
-        <v>-0.2676</v>
+        <v>-3.5799999999999998E-2</v>
       </c>
       <c r="I13" s="2">
-        <v>-0.03</v>
+        <v>8.5500000000000007E-2</v>
       </c>
       <c r="J13" s="2">
-        <v>-0.16950000000000001</v>
+        <v>-6.6699999999999995E-2</v>
       </c>
       <c r="K13" s="2">
-        <v>0.14510000000000001</v>
+        <v>0.1024</v>
       </c>
       <c r="L13" s="2">
-        <v>-0.4672</v>
+        <v>-3.7499999999999999E-2</v>
       </c>
       <c r="M13" s="2">
-        <v>1.1000000000000001E-3</v>
+        <v>0.10290000000000001</v>
       </c>
       <c r="N13" s="2">
-        <v>-0.31609999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3.2800000000000003E-2</v>
-      </c>
-      <c r="D14" s="2">
-        <v>-4.2700000000000002E-2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-9.0800000000000006E-2</v>
-      </c>
-      <c r="F14" s="2">
-        <v>-7.1499999999999994E-2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>-2.69E-2</v>
-      </c>
-      <c r="H14" s="2">
-        <v>-6.4299999999999996E-2</v>
-      </c>
-      <c r="I14" s="2">
-        <v>-2.9600000000000001E-2</v>
-      </c>
-      <c r="J14" s="2">
-        <v>-6.9099999999999995E-2</v>
-      </c>
-      <c r="K14" s="2">
-        <v>-1.35E-2</v>
-      </c>
-      <c r="L14" s="2">
-        <v>-4.1000000000000003E-3</v>
-      </c>
-      <c r="M14" s="2">
-        <v>-1.15E-2</v>
-      </c>
-      <c r="N14" s="2">
-        <v>-2.3800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-1.0800000000000001E-2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-2.35E-2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>4.5400000000000003E-2</v>
-      </c>
-      <c r="F15" s="2">
-        <v>-1.4E-3</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-5.7999999999999996E-3</v>
-      </c>
-      <c r="H15" s="2">
-        <v>-3.5799999999999998E-2</v>
-      </c>
-      <c r="I15" s="2">
-        <v>8.5500000000000007E-2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>-6.6699999999999995E-2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0.1024</v>
-      </c>
-      <c r="L15" s="2">
-        <v>-3.7499999999999999E-2</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0.10290000000000001</v>
-      </c>
-      <c r="N15" s="2">
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>